<commit_message>
updated test plan for Will
</commit_message>
<xml_diff>
--- a/EduPoll_TestPlan.xlsx
+++ b/EduPoll_TestPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wgarbutt/Documents/Documents_thismac/third_year/cosc_310/the-project-project-ricky/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/the-project-project-ricky/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCC0AF5-C70E-1945-A97D-C15C7C3320F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59666659-7817-B745-B5CB-D193FC46D07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="70">
   <si>
     <t>REQUIREMENTS</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>An user will be able to view courses they are apart of (signed in)</t>
+  </si>
+  <si>
+    <t>WG</t>
   </si>
 </sst>
 </file>
@@ -496,6 +499,60 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="4" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -519,60 +576,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -882,7 +885,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -901,10 +904,10 @@
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
@@ -916,52 +919,52 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="13" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="31" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
     </row>
     <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
     </row>
     <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
     </row>
     <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
@@ -971,19 +974,19 @@
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="17"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="21"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -1040,10 +1043,10 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="34">
+      <c r="A15" s="16">
         <v>1.4</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="12" t="s">
         <v>61</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -1057,10 +1060,10 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="34">
+      <c r="A16" s="16">
         <v>1.5</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -1074,10 +1077,10 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="34">
+      <c r="A17" s="16">
         <v>1.6</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="12" t="s">
         <v>68</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -1091,10 +1094,10 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="23"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1126,10 +1129,12 @@
       <c r="C20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="6"/>
+      <c r="D20" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
@@ -1142,10 +1147,10 @@
         <v>19</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1183,10 +1188,10 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="33">
+      <c r="A24" s="15">
         <v>2.4</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="14" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -1200,10 +1205,10 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="25"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -1260,10 +1265,10 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="31">
+      <c r="A29" s="13">
         <v>3.4</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="6" t="s">
@@ -1277,10 +1282,10 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="25"/>
+      <c r="B30" s="21"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -1316,10 +1321,10 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="28">
+      <c r="A33" s="10">
         <v>4.3</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C33" s="6"/>
@@ -1331,19 +1336,19 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="27"/>
+      <c r="B34" s="19"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
     <row r="35" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="25"/>
+      <c r="B35" s="21"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -1366,10 +1371,10 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="33">
+      <c r="A37" s="15">
         <v>1.2</v>
       </c>
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="14" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="6" t="s">
@@ -1383,19 +1388,19 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="25"/>
+      <c r="B38" s="21"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
     <row r="39" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="33">
+      <c r="A39" s="15">
         <v>2.1</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="14" t="s">
         <v>38</v>
       </c>
       <c r="C39" s="6" t="s">
@@ -1409,19 +1414,19 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="24" t="s">
+      <c r="A40" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="25"/>
+      <c r="B40" s="21"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
     <row r="41" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="33">
+      <c r="A41" s="15">
         <v>3.1</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="14" t="s">
         <v>41</v>
       </c>
       <c r="C41" s="6" t="s">
@@ -1435,19 +1440,19 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
     <row r="43" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="33">
+      <c r="A43" s="15">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B43" s="32" t="s">
+      <c r="B43" s="14" t="s">
         <v>43</v>
       </c>
       <c r="C43" s="6" t="s">
@@ -1461,10 +1466,10 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="24" t="s">
+      <c r="A44" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="25"/>
+      <c r="B44" s="21"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
@@ -1487,10 +1492,10 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="28">
+      <c r="A46" s="10">
         <v>5.2</v>
       </c>
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C46" s="6" t="s">
@@ -1504,19 +1509,19 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="s">
+      <c r="A47" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="25"/>
+      <c r="B47" s="21"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
     <row r="48" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="34">
+      <c r="A48" s="16">
         <v>6.1</v>
       </c>
-      <c r="B48" s="30" t="s">
+      <c r="B48" s="12" t="s">
         <v>48</v>
       </c>
       <c r="C48" s="6" t="s">
@@ -1530,19 +1535,19 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="25"/>
+      <c r="B49" s="21"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
     <row r="50" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="34">
+      <c r="A50" s="16">
         <v>7.1</v>
       </c>
-      <c r="B50" s="30" t="s">
+      <c r="B50" s="12" t="s">
         <v>50</v>
       </c>
       <c r="C50" s="6" t="s">
@@ -1556,10 +1561,10 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="24" t="s">
+      <c r="A51" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="25"/>
+      <c r="B51" s="21"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
@@ -1599,10 +1604,10 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="34">
+      <c r="A54" s="16">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B54" s="30" t="s">
+      <c r="B54" s="12" t="s">
         <v>54</v>
       </c>
       <c r="C54" s="6" t="s">
@@ -1633,10 +1638,10 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="18" t="s">
+      <c r="A56" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="19"/>
+      <c r="B56" s="23"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
@@ -1659,10 +1664,10 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="24" t="s">
+      <c r="A58" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B58" s="25"/>
+      <c r="B58" s="21"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
@@ -1688,11 +1693,13 @@
     <row r="61" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="E3:E8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A2:B8"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="D3:D8"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="A58:B58"/>
@@ -1701,13 +1708,11 @@
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A2:B8"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="E3:E8"/>
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A49:B49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>